<commit_message>
[Document, Modified]: Handle design for ManageProject
</commit_message>
<xml_diff>
--- a/ToDoApp-Doc/Document/Diagram/Thiết Kế Phần Mềm/Thiết Kế Xử Lý/ManageProject/Thiết kế xử lý.xlsx
+++ b/ToDoApp-Doc/Document/Diagram/Thiết Kế Phần Mềm/Thiết Kế Xử Lý/ManageProject/Thiết kế xử lý.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="172">
   <si>
     <t xml:space="preserve">DANH SÁCH CÁC KIỂU DỮ LIỆU XỬ LÝ</t>
   </si>
@@ -82,44 +82,25 @@
     <t xml:space="preserve">Thuật Giải</t>
   </si>
   <si>
+    <t xml:space="preserve">int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Số lượng project</t>
+  </si>
+  <si>
     <t xml:space="preserve">projectId</t>
   </si>
   <si>
     <t xml:space="preserve">String</t>
   </si>
   <si>
-    <t xml:space="preserve">Lưu mã project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">onToggleForm()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N/A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thực hiện việc đóng
-mở form luân phiên</t>
-  </si>
-  <si>
-    <t xml:space="preserve">int</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Số lượng project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">project_id</t>
-  </si>
-  <si>
     <t xml:space="preserve">Phải là duy nhất</t>
   </si>
   <si>
-    <t xml:space="preserve">PJ00001</t>
+    <t xml:space="preserve">null</t>
   </si>
   <si>
-    <t xml:space="preserve">projectName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lưu tên project</t>
+    <t xml:space="preserve">Lưu mã project</t>
   </si>
   <si>
     <t xml:space="preserve">LIST_PROJECT</t>
@@ -131,17 +112,14 @@
     <t xml:space="preserve">Định nghĩa hành động hiển thị danh sách các project</t>
   </si>
   <si>
-    <t xml:space="preserve">onSetProject()</t>
+    <t xml:space="preserve">toggleForm()</t>
   </si>
   <si>
-    <t xml:space="preserve">e</t>
+    <t xml:space="preserve">N/A</t>
   </si>
   <si>
-    <t xml:space="preserve">Tên project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Đặt lại gía trị cần cập
-Nhập</t>
+    <t xml:space="preserve">Thực hiện việc đóng
+mở form luân phiên</t>
   </si>
   <si>
     <t xml:space="preserve">string</t>
@@ -154,23 +132,17 @@
 - tên của project</t>
   </si>
   <si>
-    <t xml:space="preserve">user_id</t>
+    <t xml:space="preserve">userId</t>
   </si>
   <si>
     <t xml:space="preserve">Tham chiếu tới user_id
 Của class User</t>
   </si>
   <si>
-    <t xml:space="preserve">US00001</t>
+    <t xml:space="preserve">projectName</t>
   </si>
   <si>
-    <t xml:space="preserve">arrayProject</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List&lt;Project&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lưu danh sách project</t>
+    <t xml:space="preserve">Lưu tên project</t>
   </si>
   <si>
     <t xml:space="preserve">SAVE_PROJECT</t>
@@ -186,16 +158,20 @@
 cả việc thêm và sửa project</t>
   </si>
   <si>
-    <t xml:space="preserve">onExit()</t>
+    <t xml:space="preserve">setProject()</t>
   </si>
   <si>
-    <t xml:space="preserve">Đóng form</t>
+    <t xml:space="preserve">e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tên project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Đặt lại gía trị cần cập
+Nhập</t>
   </si>
   <si>
     <t xml:space="preserve">double</t>
-  </si>
-  <si>
-    <t xml:space="preserve">project_name</t>
   </si>
   <si>
     <t xml:space="preserve">Rỗng</t>
@@ -203,6 +179,36 @@
   <si>
     <t xml:space="preserve">Không được trùng với 
 project_name đã tồn tại</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arrayProject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List&lt;Project&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lưu danh sách project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DELETE_PROJECT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“deleteProject”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Định nghĩa hành động xóa project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exit()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Đóng form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Danh sách các project</t>
   </si>
   <si>
     <t xml:space="preserve">projectCreateDate</t>
@@ -214,23 +220,23 @@
     <t xml:space="preserve">Lưu ngày tạo project</t>
   </si>
   <si>
-    <t xml:space="preserve">DELETE_PROJECT</t>
+    <t xml:space="preserve">TOGGLE_FORM</t>
   </si>
   <si>
-    <t xml:space="preserve">“deleteProject”</t>
+    <t xml:space="preserve">“toggleForm”</t>
   </si>
   <si>
-    <t xml:space="preserve">Định nghĩa hành động xóa project</t>
+    <t xml:space="preserve">Định nghĩa hành động đóng mở form luân phiên</t>
   </si>
   <si>
-    <t xml:space="preserve">onSubmitForm()</t>
+    <t xml:space="preserve">submitForm()</t>
   </si>
   <si>
     <t xml:space="preserve">Project mới sau khi
 đã thêm</t>
   </si>
   <si>
-    <t xml:space="preserve">push vào List&lt;Project&gt;</t>
+    <t xml:space="preserve">push</t>
   </si>
   <si>
     <t xml:space="preserve">Thêm mới 1 project</t>
@@ -240,33 +246,6 @@
 được trùng</t>
   </si>
   <si>
-    <t xml:space="preserve">List</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Danh sách các project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">projectDeleteDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lưu ngày xóa project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOGGLE_FORM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“toggleForm”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Định nghĩa hành động đóng mở form luân phiên</t>
-  </si>
-  <si>
-    <t xml:space="preserve">onCLearForm()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Xóa thông tin trên form</t>
-  </si>
-  <si>
     <t xml:space="preserve">boolean</t>
   </si>
   <si>
@@ -274,13 +253,10 @@
 - Trạng thái của project</t>
   </si>
   <si>
-    <t xml:space="preserve">projectDao</t>
+    <t xml:space="preserve">projectDeleteDate</t>
   </si>
   <si>
-    <t xml:space="preserve">ProjectDAO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kết nối xuống lớp DAO</t>
+    <t xml:space="preserve">Lưu ngày xóa project</t>
   </si>
   <si>
     <t xml:space="preserve">OPEN_FORM</t>
@@ -292,17 +268,10 @@
     <t xml:space="preserve">Định nghĩa hành động mở form</t>
   </si>
   <si>
-    <t xml:space="preserve">onSetStatus()</t>
+    <t xml:space="preserve">cLearForm()</t>
   </si>
   <si>
-    <t xml:space="preserve">Trạng thái mới của project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vét cạn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thay đổi trạng thái
-của project</t>
+    <t xml:space="preserve">Xóa thông tin trên form</t>
   </si>
   <si>
     <t xml:space="preserve">Set</t>
@@ -318,10 +287,13 @@
     <t xml:space="preserve">DANH SÁCH CÁC THUỘC TÍNH KIỂU DỮ LIỆU Int</t>
   </si>
   <si>
-    <t xml:space="preserve">numberOfProject</t>
+    <t xml:space="preserve">projectDao</t>
   </si>
   <si>
-    <t xml:space="preserve">Lưu số lượng project trong danh sách</t>
+    <t xml:space="preserve">ProjectDAO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kết nối xuống lớp DAO</t>
   </si>
   <si>
     <t xml:space="preserve">CLOSE_FORM</t>
@@ -333,16 +305,47 @@
     <t xml:space="preserve">ĐỊnh nghĩa hành động đóng form</t>
   </si>
   <si>
-    <t xml:space="preserve">onDeleteProject()</t>
+    <t xml:space="preserve">setStatus()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trạng thái mới của project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vét cạn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thay đổi trạng thái
+của project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HashMap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numberOfProject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lưu số lượng project trong danh sách</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEARCH_FORM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“searchForm”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Định nghĩa hành động tìm kiếm project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deleteProject()</t>
   </si>
   <si>
     <t xml:space="preserve">Xóa đi 1 project</t>
   </si>
   <si>
-    <t xml:space="preserve">HashMap</t>
+    <t xml:space="preserve">Time</t>
   </si>
   <si>
-    <t xml:space="preserve">IsDisplay</t>
+    <t xml:space="preserve">isDisplay</t>
   </si>
   <si>
     <t xml:space="preserve">Lưu trạng thái đóng mở form</t>
@@ -352,13 +355,10 @@
 false là đóng</t>
   </si>
   <si>
-    <t xml:space="preserve">SEARCH_FORM</t>
+    <t xml:space="preserve">PROJECT_MAX</t>
   </si>
   <si>
-    <t xml:space="preserve">“searchForm”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Định nghĩa hành động tìm kiếm project</t>
+    <t xml:space="preserve">Số lượng project tối đa được tạo</t>
   </si>
   <si>
     <t xml:space="preserve">stateToProps()</t>
@@ -374,16 +374,14 @@
 store lên để sử dụng</t>
   </si>
   <si>
-    <t xml:space="preserve">Time</t>
+    <t xml:space="preserve">- Ngày tạo project
+- Ngày xóa project </t>
   </si>
   <si>
-    <t xml:space="preserve">number_of_project</t>
+    <t xml:space="preserve">PROJECT_NAME_MAX</t>
   </si>
   <si>
-    <t xml:space="preserve">PROJECT_MAX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Số lượng project tối đa được tạo</t>
+    <t xml:space="preserve">Số lượng ký tự tối đa của tên project</t>
   </si>
   <si>
     <t xml:space="preserve">dispatchToProps()</t>
@@ -400,52 +398,102 @@
 của người dùng</t>
   </si>
   <si>
-    <t xml:space="preserve">- Ngày tạo project
-- Ngày xóa project </t>
+    <t xml:space="preserve">PROJECT_NAME_MIN</t>
   </si>
   <si>
-    <t xml:space="preserve">PROJECT_NAME_MAX</t>
+    <t xml:space="preserve">Số lượng ký tự tối thiểu của tên project</t>
   </si>
   <si>
-    <t xml:space="preserve">Số lượng ký tự tối đa của tên project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ProjectDAO()</t>
+    <t xml:space="preserve">projectDAO()</t>
   </si>
   <si>
     <t xml:space="preserve">Constructor khởi tạo
 không chứa tham số</t>
   </si>
   <si>
-    <t xml:space="preserve">PROJECT_NAME_MIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Số lượng ký tự tối thiểu của tên project</t>
-  </si>
-  <si>
     <t xml:space="preserve">DANH SÁCH CÁC THUỘC TÍNH KIỂU DỮ LIỆU Date</t>
   </si>
   <si>
-    <t xml:space="preserve">project_created_date</t>
+    <t xml:space="preserve">timKiemDanhSachProject()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Danh sách project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lấy toàn bộ danh sách project
+Hiển thị lên cho người dùng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">truyVanDanhSachProject()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lấy toàn bộ danh sách project 
+Hiển thị lên cho người dùng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">projectCreatedDate</t>
   </si>
   <si>
     <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">null</t>
   </si>
   <si>
     <t xml:space="preserve">Phải đúng định dạng 
 Ngày tháng năm</t>
   </si>
   <si>
-    <t xml:space="preserve">project_deleted_date</t>
+    <t xml:space="preserve">renderProjects()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">projectDeletedDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kiemTraHopLe()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">true/false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kiểm tra xem tên project có bị
+trùng với tên project đã tồn tại không</t>
+  </si>
+  <si>
+    <t xml:space="preserve">getProjectName()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nhận tên project dược chuyển
+xuống từ UI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addProject()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thêm mới 1 project vào List&lt;project&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">DANH SÁCH CÁC THUỘC TÍNH KIỂU DỮ LIỆU boolean</t>
   </si>
   <si>
-    <t xml:space="preserve">project_status_id</t>
+    <t xml:space="preserve">isMoreAction()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bắt sự kiện người dùng nhấp vào
+“More actions”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">renderDanhMuc()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Danh mục các tùy chọn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hiển thị danh mục các
+Tùy chọn cho người dùng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">projectStatusId</t>
   </si>
   <si>
     <t xml:space="preserve">false</t>
@@ -455,10 +503,61 @@
 false là xóa mềm</t>
   </si>
   <si>
+    <t xml:space="preserve">isUpdate()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bắt sự kiện người dùng nhấp vào
+“Update”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">getUpdateProjectName()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id, name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lấy tên project mới</t>
+  </si>
+  <si>
+    <t xml:space="preserve">updateProject()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">project mới </t>
+  </si>
+  <si>
+    <t xml:space="preserve">nhị phân</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cập nhật lại tên project mới dưới database</t>
+  </si>
+  <si>
     <t xml:space="preserve">DANH SÁCH CÁC THUỘC TÍNH KIỂU DỮ LIỆU List&lt;Project&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">array_of_project</t>
+    <t xml:space="preserve">isDelete()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kiểm tra xem project có bị
+Người dùng xóa không</t>
+  </si>
+  <si>
+    <t xml:space="preserve">getIdDelete()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nhận id của project bị xóa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arrayOfProject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Danh sách project mới</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xóa project dưới database dựa
+vào id của project</t>
   </si>
   <si>
     <t xml:space="preserve">DANH SÁCH CÁC THUỘC TÍNH KIỂU DỮ LIỆU ProjectDAO</t>
@@ -638,7 +737,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -667,6 +766,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -684,15 +787,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -704,6 +803,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -719,20 +826,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -741,10 +840,6 @@
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -782,11 +877,11 @@
   </sheetPr>
   <dimension ref="A1:AF1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Y1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z1" activeCellId="0" sqref="Z1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Y18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AE28" activeCellId="0" sqref="AE28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36.54"/>
@@ -802,18 +897,18 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="29.31"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="17" style="1" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="13.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="13.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="28.34"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="22" min="21" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="49.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="28.48"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="26" min="25" style="1" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="22.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="31.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="16.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="26.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="25.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="22.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="21.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="40.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="28.2"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="33" style="1" width="14.43"/>
   </cols>
   <sheetData>
@@ -952,621 +1047,637 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
+      <c r="A3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="7"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
+      <c r="F3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="7"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="7" t="n">
+      <c r="M3" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="N3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="P3" s="8" t="s">
+      <c r="N3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" s="8"/>
+      <c r="O3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" s="9"/>
       <c r="R3" s="3"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
-      <c r="W3" s="5"/>
-      <c r="X3" s="5"/>
+      <c r="S3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="W3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="X3" s="7"/>
       <c r="Y3" s="3"/>
-      <c r="Z3" s="9" t="n">
+      <c r="Z3" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="AA3" s="9" t="s">
+      <c r="AA3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE3" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF3" s="10"/>
+    </row>
+    <row r="4" customFormat="false" ht="67.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="AB3" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC3" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="AD3" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="AE3" s="10" t="s">
+      <c r="I4" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AF3" s="9"/>
-    </row>
-    <row r="4" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="11"/>
+      <c r="K4" s="7"/>
       <c r="L4" s="3"/>
-      <c r="M4" s="12" t="n">
+      <c r="M4" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="N4" s="12" t="s">
+      <c r="N4" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="O4" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="W4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="X4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA4" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC4" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD4" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="O4" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="P4" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="T4" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="U4" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="V4" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="W4" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="AA4" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB4" s="9" t="s">
+      <c r="AE4" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF4" s="10"/>
+    </row>
+    <row r="5" customFormat="false" ht="66.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="AC4" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD4" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="AE4" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF4" s="9"/>
-    </row>
-    <row r="5" customFormat="false" ht="66.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="11" t="n">
-        <v>2</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="K5" s="11"/>
+      <c r="H5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>49</v>
+      </c>
       <c r="L5" s="3"/>
       <c r="M5" s="14" t="n">
         <v>3</v>
       </c>
       <c r="N5" s="15" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="O5" s="14" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="P5" s="16" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="Q5" s="16"/>
       <c r="R5" s="3"/>
-      <c r="S5" s="11" t="n">
-        <v>2</v>
-      </c>
-      <c r="T5" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="U5" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="V5" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="W5" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="X5" s="13" t="s">
-        <v>51</v>
-      </c>
+      <c r="S5" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="U5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="V5" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="W5" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="X5" s="7"/>
       <c r="Y5" s="3"/>
-      <c r="Z5" s="9" t="n">
+      <c r="Z5" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="AA5" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB5" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC5" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="AD5" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="AE5" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF5" s="9"/>
+      <c r="AA5" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE5" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="n">
-        <v>3</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
+      <c r="A6" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="7"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="11" t="n">
-        <v>3</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="K6" s="13" t="s">
-        <v>57</v>
-      </c>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="18"/>
       <c r="L6" s="3"/>
-      <c r="M6" s="17" t="n">
+      <c r="M6" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="N6" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="O6" s="19" t="s">
-        <v>59</v>
+      <c r="N6" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="O6" s="21" t="s">
+        <v>61</v>
       </c>
       <c r="P6" s="16" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="Q6" s="16"/>
       <c r="R6" s="3"/>
-      <c r="S6" s="11" t="n">
-        <v>3</v>
-      </c>
-      <c r="T6" s="11" t="s">
+      <c r="S6" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="T6" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="U6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="V6" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="W6" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA6" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC6" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD6" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE6" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF6" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="19" t="n">
+        <v>5</v>
+      </c>
+      <c r="N7" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="O7" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="U6" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="V6" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="W6" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="X6" s="11"/>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="9" t="n">
-        <v>4</v>
-      </c>
-      <c r="AA6" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="AB6" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC6" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD6" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE6" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="AF6" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="n">
-        <v>4</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="17" t="n">
-        <v>5</v>
-      </c>
-      <c r="N7" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="O7" s="19" t="s">
-        <v>59</v>
-      </c>
       <c r="P7" s="16" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="Q7" s="16"/>
       <c r="R7" s="3"/>
-      <c r="S7" s="11" t="n">
-        <v>4</v>
-      </c>
-      <c r="T7" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="U7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="V7" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="W7" s="11" t="s">
+      <c r="S7" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="T7" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="X7" s="11"/>
+      <c r="U7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="V7" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="W7" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="X7" s="7"/>
       <c r="Y7" s="3"/>
-      <c r="Z7" s="9" t="n">
+      <c r="Z7" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="AA7" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="AB7" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC7" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="AD7" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="AE7" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="AF7" s="9"/>
+      <c r="AA7" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE7" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="n">
-        <v>5</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8" s="11"/>
+      <c r="A8" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>82</v>
+      </c>
       <c r="E8" s="3"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="21"/>
+      <c r="F8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
       <c r="L8" s="3"/>
       <c r="M8" s="14" t="n">
         <v>6</v>
       </c>
       <c r="N8" s="14" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="O8" s="14" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="P8" s="16" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="Q8" s="16"/>
       <c r="R8" s="3"/>
-      <c r="S8" s="11" t="n">
+      <c r="S8" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="T8" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="U8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="V8" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="W8" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="AA8" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC8" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD8" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="AE8" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF8" s="10"/>
+    </row>
+    <row r="9" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="T8" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="U8" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="V8" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="W8" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="X8" s="11"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="AA8" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="AB8" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC8" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="AD8" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="AE8" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="AF8" s="9"/>
-    </row>
-    <row r="9" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="n">
-        <v>6</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
+      <c r="G9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="L9" s="3"/>
       <c r="M9" s="16" t="n">
         <v>7</v>
       </c>
       <c r="N9" s="16" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="O9" s="16" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="P9" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q9" s="16"/>
       <c r="R9" s="3"/>
-      <c r="S9" s="11" t="n">
-        <v>6</v>
-      </c>
-      <c r="T9" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="U9" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="V9" s="11" t="s">
+      <c r="S9" s="7" t="n">
+        <v>7</v>
+      </c>
+      <c r="T9" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="W9" s="11" t="s">
+      <c r="U9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="V9" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="X9" s="11"/>
+      <c r="W9" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="X9" s="7"/>
       <c r="Y9" s="3"/>
-      <c r="Z9" s="9" t="n">
+      <c r="Z9" s="10" t="n">
         <v>7</v>
       </c>
-      <c r="AA9" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="AB9" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC9" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="AD9" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="AE9" s="9" t="s">
+      <c r="AA9" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="AF9" s="9"/>
+      <c r="AB9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD9" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="AE9" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="AF9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="n">
-        <v>7</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+      <c r="A10" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" s="5" t="s">
+      <c r="F10" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="12"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="13" t="n">
+        <v>8</v>
+      </c>
+      <c r="N10" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="O10" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="P10" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q10" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="R10" s="3"/>
+      <c r="S10" s="23" t="n">
+        <v>8</v>
+      </c>
+      <c r="T10" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="U10" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="V10" s="23" t="n">
+        <v>1000</v>
+      </c>
+      <c r="W10" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="X10" s="23"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA10" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="AB10" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC10" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="AD10" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE10" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF10" s="10"/>
+    </row>
+    <row r="11" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="H10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="L10" s="3"/>
-      <c r="M10" s="22" t="n">
-        <v>8</v>
-      </c>
-      <c r="N10" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="O10" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="P10" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q10" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="R10" s="3"/>
-      <c r="S10" s="11" t="n">
-        <v>7</v>
-      </c>
-      <c r="T10" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="U10" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="V10" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="W10" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="X10" s="11"/>
-      <c r="Y10" s="3"/>
-      <c r="Z10" s="9" t="n">
-        <v>8</v>
-      </c>
-      <c r="AA10" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="AB10" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="AC10" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="AD10" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="AE10" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF10" s="9"/>
-    </row>
-    <row r="11" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11" t="n">
-        <v>8</v>
-      </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
+      <c r="D11" s="7"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" s="13"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="18"/>
       <c r="L11" s="3"/>
       <c r="M11" s="24"/>
       <c r="N11" s="24"/>
@@ -1574,61 +1685,55 @@
       <c r="P11" s="25"/>
       <c r="Q11" s="25"/>
       <c r="R11" s="3"/>
-      <c r="S11" s="26" t="n">
-        <v>8</v>
-      </c>
-      <c r="T11" s="26" t="s">
+      <c r="S11" s="23" t="n">
+        <v>9</v>
+      </c>
+      <c r="T11" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="U11" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="V11" s="23" t="n">
+        <v>1000</v>
+      </c>
+      <c r="W11" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="U11" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="V11" s="26" t="n">
-        <v>1000</v>
-      </c>
-      <c r="W11" s="26" t="s">
+      <c r="X11" s="23"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="10" t="n">
+        <v>9</v>
+      </c>
+      <c r="AA11" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="X11" s="26"/>
-      <c r="Y11" s="3"/>
-      <c r="Z11" s="9" t="n">
-        <v>9</v>
-      </c>
-      <c r="AA11" s="9" t="s">
+      <c r="AB11" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="AB11" s="9" t="s">
+      <c r="AC11" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="AC11" s="10" t="s">
+      <c r="AD11" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE11" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="AD11" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="AE11" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="AF11" s="9"/>
+      <c r="AF11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11" t="n">
-        <v>9</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="D12" s="11"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="21"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
       <c r="L12" s="3"/>
       <c r="M12" s="0"/>
       <c r="N12" s="0"/>
@@ -1636,55 +1741,57 @@
       <c r="P12" s="0"/>
       <c r="Q12" s="0"/>
       <c r="R12" s="3"/>
-      <c r="S12" s="26" t="n">
-        <v>9</v>
-      </c>
-      <c r="T12" s="26" t="s">
+      <c r="S12" s="23" t="n">
+        <v>10</v>
+      </c>
+      <c r="T12" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="U12" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="V12" s="23" t="n">
+        <v>5</v>
+      </c>
+      <c r="W12" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="X12" s="23"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="10" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA12" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="U12" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="V12" s="26" t="n">
-        <v>1000</v>
-      </c>
-      <c r="W12" s="26" t="s">
+      <c r="AB12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE12" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="X12" s="26"/>
-      <c r="Y12" s="3"/>
-      <c r="Z12" s="9" t="n">
-        <v>10</v>
-      </c>
-      <c r="AA12" s="9" t="s">
+      <c r="AF12" s="10"/>
+    </row>
+    <row r="13" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AB12" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC12" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="AD12" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="AE12" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="AF12" s="9"/>
-    </row>
-    <row r="13" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="20"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
       <c r="L13" s="3"/>
       <c r="M13" s="0"/>
       <c r="N13" s="0"/>
@@ -1692,45 +1799,57 @@
       <c r="P13" s="0"/>
       <c r="Q13" s="0"/>
       <c r="R13" s="3"/>
-      <c r="S13" s="26" t="n">
-        <v>10</v>
-      </c>
-      <c r="T13" s="26" t="s">
-        <v>125</v>
-      </c>
-      <c r="U13" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="V13" s="26" t="n">
-        <v>5</v>
-      </c>
-      <c r="W13" s="26" t="s">
-        <v>126</v>
-      </c>
+      <c r="S13" s="26"/>
+      <c r="T13" s="26"/>
+      <c r="U13" s="26"/>
+      <c r="V13" s="26"/>
+      <c r="W13" s="26"/>
       <c r="X13" s="26"/>
       <c r="Y13" s="3"/>
-      <c r="Z13" s="27"/>
-      <c r="AA13" s="28"/>
-      <c r="AB13" s="28"/>
-      <c r="AC13" s="28"/>
-      <c r="AD13" s="28"/>
-      <c r="AE13" s="28"/>
-      <c r="AF13" s="28"/>
+      <c r="Z13" s="13" t="n">
+        <v>11</v>
+      </c>
+      <c r="AA13" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB13" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC13" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="AD13" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="AE13" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="AF13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
+      <c r="F14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="L14" s="3"/>
       <c r="M14" s="0"/>
       <c r="N14" s="0"/>
@@ -1738,20 +1857,32 @@
       <c r="P14" s="0"/>
       <c r="Q14" s="0"/>
       <c r="R14" s="3"/>
-      <c r="S14" s="27"/>
-      <c r="T14" s="27"/>
-      <c r="U14" s="27"/>
-      <c r="V14" s="27"/>
-      <c r="W14" s="27"/>
-      <c r="X14" s="27"/>
+      <c r="S14" s="26"/>
+      <c r="T14" s="26"/>
+      <c r="U14" s="26"/>
+      <c r="V14" s="26"/>
+      <c r="W14" s="26"/>
+      <c r="X14" s="26"/>
       <c r="Y14" s="3"/>
-      <c r="Z14" s="27"/>
-      <c r="AA14" s="28"/>
-      <c r="AB14" s="28"/>
-      <c r="AC14" s="28"/>
-      <c r="AD14" s="28"/>
-      <c r="AE14" s="28"/>
-      <c r="AF14" s="28"/>
+      <c r="Z14" s="13" t="n">
+        <v>12</v>
+      </c>
+      <c r="AA14" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB14" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC14" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="AD14" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="AE14" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="AF14" s="13"/>
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3"/>
@@ -1759,23 +1890,21 @@
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>8</v>
+      <c r="F15" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>131</v>
       </c>
       <c r="L15" s="3"/>
       <c r="M15" s="0"/>
@@ -1784,20 +1913,30 @@
       <c r="P15" s="0"/>
       <c r="Q15" s="0"/>
       <c r="R15" s="3"/>
-      <c r="S15" s="27"/>
-      <c r="T15" s="27"/>
-      <c r="U15" s="27"/>
-      <c r="V15" s="27"/>
-      <c r="W15" s="27"/>
-      <c r="X15" s="27"/>
+      <c r="S15" s="26"/>
+      <c r="T15" s="26"/>
+      <c r="U15" s="26"/>
+      <c r="V15" s="26"/>
+      <c r="W15" s="26"/>
+      <c r="X15" s="26"/>
       <c r="Y15" s="3"/>
-      <c r="Z15" s="27"/>
-      <c r="AA15" s="28"/>
-      <c r="AB15" s="28"/>
-      <c r="AC15" s="28"/>
-      <c r="AD15" s="28"/>
-      <c r="AE15" s="28"/>
-      <c r="AF15" s="28"/>
+      <c r="Z15" s="13" t="n">
+        <v>13</v>
+      </c>
+      <c r="AA15" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="AB15" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC15" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="AD15" s="13"/>
+      <c r="AE15" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="AF15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3"/>
@@ -1805,20 +1944,20 @@
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11" t="s">
+      <c r="F16" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="H16" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="K16" s="13" t="s">
+      <c r="I16" s="12"/>
+      <c r="J16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16" s="12" t="s">
         <v>131</v>
       </c>
       <c r="L16" s="3"/>
@@ -1828,20 +1967,30 @@
       <c r="P16" s="0"/>
       <c r="Q16" s="0"/>
       <c r="R16" s="3"/>
-      <c r="S16" s="27"/>
-      <c r="T16" s="27"/>
-      <c r="U16" s="27"/>
-      <c r="V16" s="27"/>
-      <c r="W16" s="27"/>
-      <c r="X16" s="27"/>
+      <c r="S16" s="26"/>
+      <c r="T16" s="26"/>
+      <c r="U16" s="26"/>
+      <c r="V16" s="26"/>
+      <c r="W16" s="26"/>
+      <c r="X16" s="26"/>
       <c r="Y16" s="3"/>
-      <c r="Z16" s="27"/>
-      <c r="AA16" s="28"/>
-      <c r="AB16" s="28"/>
-      <c r="AC16" s="28"/>
-      <c r="AD16" s="28"/>
-      <c r="AE16" s="28"/>
-      <c r="AF16" s="28"/>
+      <c r="Z16" s="13" t="n">
+        <v>14</v>
+      </c>
+      <c r="AA16" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="AB16" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="AC16" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="AD16" s="13"/>
+      <c r="AE16" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="AF16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3"/>
@@ -1849,22 +1998,12 @@
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="11" t="n">
-        <v>2</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="I17" s="13"/>
-      <c r="J17" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="K17" s="13" t="s">
-        <v>131</v>
-      </c>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="18"/>
       <c r="L17" s="3"/>
       <c r="M17" s="0"/>
       <c r="N17" s="0"/>
@@ -1872,20 +2011,30 @@
       <c r="P17" s="0"/>
       <c r="Q17" s="0"/>
       <c r="R17" s="3"/>
-      <c r="S17" s="27"/>
-      <c r="T17" s="27"/>
-      <c r="U17" s="27"/>
-      <c r="V17" s="27"/>
-      <c r="W17" s="27"/>
-      <c r="X17" s="27"/>
+      <c r="S17" s="26"/>
+      <c r="T17" s="26"/>
+      <c r="U17" s="26"/>
+      <c r="V17" s="26"/>
+      <c r="W17" s="26"/>
+      <c r="X17" s="26"/>
       <c r="Y17" s="3"/>
-      <c r="Z17" s="27"/>
-      <c r="AA17" s="28"/>
-      <c r="AB17" s="28"/>
-      <c r="AC17" s="28"/>
-      <c r="AD17" s="28"/>
-      <c r="AE17" s="28"/>
-      <c r="AF17" s="28"/>
+      <c r="Z17" s="13" t="n">
+        <v>15</v>
+      </c>
+      <c r="AA17" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="AB17" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC17" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD17" s="13"/>
+      <c r="AE17" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="AF17" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3"/>
@@ -1893,12 +2042,12 @@
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="21"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="18"/>
       <c r="L18" s="3"/>
       <c r="M18" s="24"/>
       <c r="N18" s="24"/>
@@ -1906,20 +2055,32 @@
       <c r="P18" s="25"/>
       <c r="Q18" s="25"/>
       <c r="R18" s="3"/>
-      <c r="S18" s="27"/>
-      <c r="T18" s="27"/>
-      <c r="U18" s="27"/>
-      <c r="V18" s="27"/>
-      <c r="W18" s="27"/>
-      <c r="X18" s="27"/>
+      <c r="S18" s="26"/>
+      <c r="T18" s="26"/>
+      <c r="U18" s="26"/>
+      <c r="V18" s="26"/>
+      <c r="W18" s="26"/>
+      <c r="X18" s="26"/>
       <c r="Y18" s="3"/>
-      <c r="Z18" s="27"/>
-      <c r="AA18" s="28"/>
-      <c r="AB18" s="28"/>
-      <c r="AC18" s="28"/>
-      <c r="AD18" s="28"/>
-      <c r="AE18" s="28"/>
-      <c r="AF18" s="28"/>
+      <c r="Z18" s="13" t="n">
+        <v>16</v>
+      </c>
+      <c r="AA18" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB18" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="AC18" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="AD18" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE18" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="AF18" s="13"/>
     </row>
     <row r="19" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="3"/>
@@ -1927,12 +2088,14 @@
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="21"/>
+      <c r="F19" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
       <c r="L19" s="3"/>
       <c r="M19" s="24"/>
       <c r="N19" s="24"/>
@@ -1940,20 +2103,30 @@
       <c r="P19" s="25"/>
       <c r="Q19" s="25"/>
       <c r="R19" s="3"/>
-      <c r="S19" s="27"/>
-      <c r="T19" s="27"/>
-      <c r="U19" s="27"/>
-      <c r="V19" s="27"/>
-      <c r="W19" s="27"/>
-      <c r="X19" s="27"/>
+      <c r="S19" s="26"/>
+      <c r="T19" s="26"/>
+      <c r="U19" s="26"/>
+      <c r="V19" s="26"/>
+      <c r="W19" s="26"/>
+      <c r="X19" s="26"/>
       <c r="Y19" s="3"/>
-      <c r="Z19" s="27"/>
-      <c r="AA19" s="28"/>
-      <c r="AB19" s="28"/>
-      <c r="AC19" s="28"/>
-      <c r="AD19" s="28"/>
-      <c r="AE19" s="28"/>
-      <c r="AF19" s="28"/>
+      <c r="Z19" s="13" t="n">
+        <v>17</v>
+      </c>
+      <c r="AA19" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB19" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC19" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="AD19" s="13"/>
+      <c r="AE19" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="AF19" s="13"/>
     </row>
     <row r="20" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="3"/>
@@ -1961,14 +2134,24 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
+      <c r="F20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="L20" s="3"/>
       <c r="M20" s="24"/>
       <c r="N20" s="24"/>
@@ -1976,20 +2159,30 @@
       <c r="P20" s="25"/>
       <c r="Q20" s="25"/>
       <c r="R20" s="3"/>
-      <c r="S20" s="27"/>
-      <c r="T20" s="27"/>
-      <c r="U20" s="27"/>
-      <c r="V20" s="27"/>
-      <c r="W20" s="27"/>
-      <c r="X20" s="27"/>
+      <c r="S20" s="26"/>
+      <c r="T20" s="26"/>
+      <c r="U20" s="26"/>
+      <c r="V20" s="26"/>
+      <c r="W20" s="26"/>
+      <c r="X20" s="26"/>
       <c r="Y20" s="3"/>
-      <c r="Z20" s="27"/>
-      <c r="AA20" s="28"/>
-      <c r="AB20" s="28"/>
-      <c r="AC20" s="28"/>
-      <c r="AD20" s="28"/>
-      <c r="AE20" s="28"/>
-      <c r="AF20" s="28"/>
+      <c r="Z20" s="13" t="n">
+        <v>18</v>
+      </c>
+      <c r="AA20" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="AB20" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC20" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="AD20" s="13"/>
+      <c r="AE20" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="AF20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="3"/>
@@ -1997,23 +2190,21 @@
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K21" s="5" t="s">
-        <v>8</v>
+      <c r="F21" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="K21" s="12" t="s">
+        <v>150</v>
       </c>
       <c r="L21" s="3"/>
       <c r="M21" s="25"/>
@@ -2022,20 +2213,30 @@
       <c r="P21" s="25"/>
       <c r="Q21" s="25"/>
       <c r="R21" s="3"/>
-      <c r="S21" s="27"/>
-      <c r="T21" s="27"/>
-      <c r="U21" s="27"/>
-      <c r="V21" s="27"/>
-      <c r="W21" s="27"/>
-      <c r="X21" s="27"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
       <c r="Y21" s="3"/>
-      <c r="Z21" s="27"/>
-      <c r="AA21" s="28"/>
-      <c r="AB21" s="28"/>
-      <c r="AC21" s="28"/>
-      <c r="AD21" s="28"/>
-      <c r="AE21" s="28"/>
-      <c r="AF21" s="28"/>
+      <c r="Z21" s="13" t="n">
+        <v>19</v>
+      </c>
+      <c r="AA21" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB21" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC21" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="AD21" s="13"/>
+      <c r="AE21" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="AF21" s="13"/>
     </row>
     <row r="22" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3"/>
@@ -2043,22 +2244,12 @@
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="K22" s="13" t="s">
-        <v>136</v>
-      </c>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
       <c r="L22" s="3"/>
       <c r="M22" s="25"/>
       <c r="N22" s="25"/>
@@ -2073,13 +2264,23 @@
       <c r="W22" s="3"/>
       <c r="X22" s="3"/>
       <c r="Y22" s="3"/>
-      <c r="Z22" s="27"/>
-      <c r="AA22" s="28"/>
-      <c r="AB22" s="28"/>
-      <c r="AC22" s="28"/>
-      <c r="AD22" s="28"/>
-      <c r="AE22" s="28"/>
-      <c r="AF22" s="28"/>
+      <c r="Z22" s="13" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA22" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AB22" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="AC22" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD22" s="13"/>
+      <c r="AE22" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="AF22" s="27"/>
     </row>
     <row r="23" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="3"/>
@@ -2087,12 +2288,12 @@
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="18"/>
       <c r="L23" s="3"/>
       <c r="M23" s="25"/>
       <c r="N23" s="25"/>
@@ -2107,13 +2308,25 @@
       <c r="W23" s="3"/>
       <c r="X23" s="3"/>
       <c r="Y23" s="3"/>
-      <c r="Z23" s="27"/>
-      <c r="AA23" s="28"/>
-      <c r="AB23" s="28"/>
-      <c r="AC23" s="28"/>
-      <c r="AD23" s="28"/>
-      <c r="AE23" s="28"/>
-      <c r="AF23" s="28"/>
+      <c r="Z23" s="13" t="n">
+        <v>21</v>
+      </c>
+      <c r="AA23" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="AB23" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="AC23" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="AD23" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE23" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="AF23" s="27"/>
     </row>
     <row r="24" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="3"/>
@@ -2121,18 +2334,20 @@
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="21"/>
+      <c r="F24" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
       <c r="L24" s="3"/>
       <c r="M24" s="25"/>
       <c r="N24" s="25"/>
       <c r="O24" s="25"/>
       <c r="P24" s="25"/>
-      <c r="Q24" s="29"/>
+      <c r="Q24" s="28"/>
       <c r="R24" s="3"/>
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
@@ -2141,13 +2356,23 @@
       <c r="W24" s="3"/>
       <c r="X24" s="3"/>
       <c r="Y24" s="3"/>
-      <c r="Z24" s="27"/>
-      <c r="AA24" s="28"/>
-      <c r="AB24" s="28"/>
-      <c r="AC24" s="28"/>
-      <c r="AD24" s="28"/>
-      <c r="AE24" s="28"/>
-      <c r="AF24" s="28"/>
+      <c r="Z24" s="13" t="n">
+        <v>22</v>
+      </c>
+      <c r="AA24" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB24" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="AC24" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="AD24" s="13"/>
+      <c r="AE24" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="AF24" s="27"/>
     </row>
     <row r="25" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="3"/>
@@ -2155,14 +2380,24 @@
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
+      <c r="F25" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="L25" s="3"/>
       <c r="M25" s="0"/>
       <c r="N25" s="0"/>
@@ -2177,7 +2412,22 @@
       <c r="W25" s="3"/>
       <c r="X25" s="3"/>
       <c r="Y25" s="3"/>
-      <c r="Z25" s="3"/>
+      <c r="Z25" s="13" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA25" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="AB25" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="AC25" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD25" s="13"/>
+      <c r="AE25" s="13" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3"/>
@@ -2185,24 +2435,20 @@
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J26" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K26" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="F26" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K26" s="7"/>
       <c r="L26" s="3"/>
       <c r="M26" s="25"/>
       <c r="N26" s="25"/>
@@ -2217,7 +2463,24 @@
       <c r="W26" s="3"/>
       <c r="X26" s="3"/>
       <c r="Y26" s="3"/>
-      <c r="Z26" s="3"/>
+      <c r="Z26" s="13" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA26" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB26" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="AC26" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="AD26" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE26" s="22" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="3"/>
@@ -2225,20 +2488,12 @@
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="K27" s="11"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
       <c r="L27" s="3"/>
       <c r="M27" s="24"/>
       <c r="N27" s="24"/>
@@ -2261,12 +2516,12 @@
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
+      <c r="K28" s="18"/>
       <c r="L28" s="3"/>
       <c r="M28" s="24"/>
       <c r="N28" s="24"/>
@@ -2289,12 +2544,14 @@
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="21"/>
+      <c r="F29" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
       <c r="L29" s="3"/>
       <c r="M29" s="24"/>
       <c r="N29" s="24"/>
@@ -2317,14 +2574,24 @@
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
-      <c r="F30" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
+      <c r="F30" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="L30" s="3"/>
       <c r="M30" s="24"/>
       <c r="N30" s="24"/>
@@ -2347,23 +2614,21 @@
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
-      <c r="F31" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I31" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J31" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K31" s="5" t="s">
-        <v>8</v>
+      <c r="F31" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="K31" s="12" t="s">
+        <v>171</v>
       </c>
       <c r="L31" s="3"/>
       <c r="M31" s="24"/>
@@ -2387,22 +2652,12 @@
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
-      <c r="F32" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="G32" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="H32" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="K32" s="13" t="s">
-        <v>141</v>
-      </c>
+      <c r="F32" s="0"/>
+      <c r="G32" s="0"/>
+      <c r="H32" s="0"/>
+      <c r="I32" s="0"/>
+      <c r="J32" s="0"/>
+      <c r="K32" s="0"/>
       <c r="L32" s="3"/>
       <c r="M32" s="24"/>
       <c r="N32" s="24"/>
@@ -2517,7 +2772,7 @@
       <c r="K36" s="0"/>
       <c r="L36" s="3"/>
       <c r="M36" s="24"/>
-      <c r="N36" s="30"/>
+      <c r="N36" s="29"/>
       <c r="O36" s="24"/>
       <c r="P36" s="25"/>
       <c r="Q36" s="25"/>
@@ -2545,7 +2800,7 @@
       <c r="K37" s="0"/>
       <c r="L37" s="3"/>
       <c r="M37" s="24"/>
-      <c r="N37" s="30"/>
+      <c r="N37" s="29"/>
       <c r="O37" s="24"/>
       <c r="P37" s="25"/>
       <c r="Q37" s="25"/>
@@ -2573,7 +2828,7 @@
       <c r="K38" s="0"/>
       <c r="L38" s="3"/>
       <c r="M38" s="24"/>
-      <c r="N38" s="30"/>
+      <c r="N38" s="29"/>
       <c r="O38" s="24"/>
       <c r="P38" s="25"/>
       <c r="Q38" s="25"/>
@@ -2761,12 +3016,12 @@
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
-      <c r="F45" s="0"/>
-      <c r="G45" s="0"/>
-      <c r="H45" s="0"/>
-      <c r="I45" s="0"/>
-      <c r="J45" s="0"/>
-      <c r="K45" s="0"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="17"/>
+      <c r="I45" s="17"/>
+      <c r="J45" s="17"/>
+      <c r="K45" s="17"/>
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
       <c r="N45" s="3"/>
@@ -2789,12 +3044,12 @@
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="20"/>
-      <c r="I46" s="20"/>
-      <c r="J46" s="20"/>
-      <c r="K46" s="20"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
+      <c r="J46" s="17"/>
+      <c r="K46" s="18"/>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
       <c r="N46" s="3"/>
@@ -2817,12 +3072,12 @@
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
-      <c r="I47" s="20"/>
-      <c r="J47" s="20"/>
-      <c r="K47" s="21"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
       <c r="N47" s="3"/>
@@ -2873,12 +3128,12 @@
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
+      <c r="F49" s="0"/>
+      <c r="G49" s="0"/>
+      <c r="H49" s="0"/>
+      <c r="I49" s="0"/>
+      <c r="J49" s="0"/>
+      <c r="K49" s="0"/>
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
       <c r="N49" s="3"/>
@@ -2957,12 +3212,12 @@
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
-      <c r="F52" s="0"/>
-      <c r="G52" s="0"/>
-      <c r="H52" s="0"/>
-      <c r="I52" s="0"/>
-      <c r="J52" s="0"/>
-      <c r="K52" s="0"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="17"/>
+      <c r="H52" s="17"/>
+      <c r="I52" s="18"/>
+      <c r="J52" s="17"/>
+      <c r="K52" s="17"/>
       <c r="L52" s="3"/>
       <c r="M52" s="3"/>
       <c r="N52" s="3"/>
@@ -2985,12 +3240,12 @@
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
-      <c r="F53" s="20"/>
-      <c r="G53" s="20"/>
-      <c r="H53" s="20"/>
-      <c r="I53" s="21"/>
-      <c r="J53" s="20"/>
-      <c r="K53" s="20"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="17"/>
+      <c r="J53" s="17"/>
+      <c r="K53" s="18"/>
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
       <c r="N53" s="3"/>
@@ -3013,12 +3268,12 @@
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
-      <c r="F54" s="20"/>
-      <c r="G54" s="20"/>
-      <c r="H54" s="20"/>
-      <c r="I54" s="20"/>
-      <c r="J54" s="20"/>
-      <c r="K54" s="21"/>
+      <c r="F54" s="17"/>
+      <c r="G54" s="17"/>
+      <c r="H54" s="17"/>
+      <c r="I54" s="17"/>
+      <c r="J54" s="17"/>
+      <c r="K54" s="18"/>
       <c r="L54" s="3"/>
       <c r="M54" s="3"/>
       <c r="N54" s="3"/>
@@ -3041,12 +3296,12 @@
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
-      <c r="F55" s="20"/>
-      <c r="G55" s="20"/>
-      <c r="H55" s="20"/>
-      <c r="I55" s="20"/>
-      <c r="J55" s="20"/>
-      <c r="K55" s="21"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="17"/>
+      <c r="H55" s="17"/>
+      <c r="I55" s="17"/>
+      <c r="J55" s="17"/>
+      <c r="K55" s="18"/>
       <c r="L55" s="3"/>
       <c r="M55" s="3"/>
       <c r="N55" s="3"/>
@@ -3069,12 +3324,12 @@
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
-      <c r="F56" s="20"/>
-      <c r="G56" s="20"/>
-      <c r="H56" s="20"/>
-      <c r="I56" s="20"/>
-      <c r="J56" s="20"/>
-      <c r="K56" s="21"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="17"/>
+      <c r="J56" s="17"/>
+      <c r="K56" s="18"/>
       <c r="L56" s="3"/>
       <c r="M56" s="3"/>
       <c r="N56" s="3"/>
@@ -3097,12 +3352,12 @@
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
-      <c r="F57" s="20"/>
-      <c r="G57" s="20"/>
-      <c r="H57" s="20"/>
-      <c r="I57" s="20"/>
-      <c r="J57" s="20"/>
-      <c r="K57" s="21"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="17"/>
+      <c r="H57" s="17"/>
+      <c r="I57" s="17"/>
+      <c r="J57" s="17"/>
+      <c r="K57" s="17"/>
       <c r="L57" s="3"/>
       <c r="M57" s="3"/>
       <c r="N57" s="3"/>
@@ -3125,12 +3380,12 @@
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
-      <c r="F58" s="20"/>
-      <c r="G58" s="20"/>
-      <c r="H58" s="20"/>
-      <c r="I58" s="20"/>
-      <c r="J58" s="20"/>
-      <c r="K58" s="20"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
+      <c r="H58" s="17"/>
+      <c r="I58" s="17"/>
+      <c r="J58" s="17"/>
+      <c r="K58" s="18"/>
       <c r="L58" s="3"/>
       <c r="M58" s="3"/>
       <c r="N58" s="3"/>
@@ -3153,12 +3408,12 @@
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
-      <c r="F59" s="20"/>
-      <c r="G59" s="20"/>
-      <c r="H59" s="20"/>
-      <c r="I59" s="20"/>
-      <c r="J59" s="20"/>
-      <c r="K59" s="21"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="3"/>
+      <c r="J59" s="3"/>
+      <c r="K59" s="3"/>
       <c r="L59" s="3"/>
       <c r="M59" s="3"/>
       <c r="N59" s="3"/>
@@ -29524,17 +29779,7 @@
       <c r="Z1000" s="3"/>
     </row>
     <row r="1001" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1001" s="3"/>
-      <c r="B1001" s="3"/>
-      <c r="C1001" s="3"/>
-      <c r="D1001" s="3"/>
       <c r="E1001" s="3"/>
-      <c r="F1001" s="3"/>
-      <c r="G1001" s="3"/>
-      <c r="H1001" s="3"/>
-      <c r="I1001" s="3"/>
-      <c r="J1001" s="3"/>
-      <c r="K1001" s="3"/>
       <c r="L1001" s="3"/>
       <c r="M1001" s="3"/>
       <c r="N1001" s="3"/>
@@ -29542,12 +29787,6 @@
       <c r="P1001" s="3"/>
       <c r="Q1001" s="3"/>
       <c r="R1001" s="3"/>
-      <c r="S1001" s="3"/>
-      <c r="T1001" s="3"/>
-      <c r="U1001" s="3"/>
-      <c r="V1001" s="3"/>
-      <c r="W1001" s="3"/>
-      <c r="X1001" s="3"/>
       <c r="Y1001" s="3"/>
       <c r="Z1001" s="3"/>
     </row>
@@ -29558,11 +29797,11 @@
     <mergeCell ref="M1:Q1"/>
     <mergeCell ref="S1:X1"/>
     <mergeCell ref="Z1:AF1"/>
-    <mergeCell ref="F9:K9"/>
-    <mergeCell ref="F14:K14"/>
-    <mergeCell ref="F20:K20"/>
-    <mergeCell ref="F25:K25"/>
-    <mergeCell ref="F30:K30"/>
+    <mergeCell ref="F8:K8"/>
+    <mergeCell ref="F13:K13"/>
+    <mergeCell ref="F19:K19"/>
+    <mergeCell ref="F24:K24"/>
+    <mergeCell ref="F29:K29"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>